<commit_message>
Neutral Point Final Labeled Graphs
</commit_message>
<xml_diff>
--- a/Lab 6/neutral moment update.xlsx
+++ b/Lab 6/neutral moment update.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\ae460\lab05_06\AE-460\Lab 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560B51E1-8430-4736-89DD-E60B5A812589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F7DEAA-70FA-4FCA-90D0-86B17BBAD0BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7DB2D3F6-6F86-4E49-8BA8-4E3C7F5D5D0B}"/>
   </bookViews>
@@ -3579,7 +3579,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Series 1</c:v>
+            <c:v>2.6 in</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -3706,7 +3706,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Series 2</c:v>
+            <c:v>2.65 in</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -3782,7 +3782,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Series 3</c:v>
+            <c:v>2.7 in</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -3858,7 +3858,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>Series 4</c:v>
+            <c:v>2.75 in</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -3934,7 +3934,7 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>Series 5</c:v>
+            <c:v>2.8 in</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -4010,7 +4010,7 @@
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
-            <c:v>Series 6</c:v>
+            <c:v>2.85 in</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -4086,7 +4086,7 @@
           <c:idx val="6"/>
           <c:order val="6"/>
           <c:tx>
-            <c:v>Series 7</c:v>
+            <c:v>2.9 in</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -4555,6 +4555,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>2.25 in</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -4692,7 +4695,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Series 2</c:v>
+            <c:v>2.3 in</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -4831,7 +4834,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Series 3</c:v>
+            <c:v>2.35 in</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -4970,7 +4973,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>Series 4</c:v>
+            <c:v>2.4 in</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -5109,7 +5112,7 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>Series 5</c:v>
+            <c:v>2.45 in</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -5248,7 +5251,7 @@
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
-            <c:v>Series 6</c:v>
+            <c:v>2.5 in</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -5387,7 +5390,7 @@
           <c:idx val="6"/>
           <c:order val="6"/>
           <c:tx>
-            <c:v>Series 7</c:v>
+            <c:v>2.55 in</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -5781,6 +5784,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -13735,16 +13769,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>696685</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>500744</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>43543</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>674914</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>87085</xdr:rowOff>
+      <xdr:colOff>674915</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>97972</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13776,16 +13810,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>11430</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>156210</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>316230</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>506730</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16114,8 +16148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBB9CFD-C2AD-D349-8BB0-705312183456}">
   <dimension ref="A1:AF62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD35" sqref="AD35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -20087,7 +20121,7 @@
   <dimension ref="A1:X56"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="W24" sqref="W24"/>
+      <selection activeCell="Z12" sqref="Z12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -23178,7 +23212,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView zoomScale="103" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Cm vs aoa graph
</commit_message>
<xml_diff>
--- a/Lab 6/neutral moment update.xlsx
+++ b/Lab 6/neutral moment update.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\ae460\lab05_06\AE-460\Lab 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD1D041-5ABB-4FC0-ABEE-96D7D8A0BE46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E828FE-3350-4098-BA99-312707622990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7DB2D3F6-6F86-4E49-8BA8-4E3C7F5D5D0B}"/>
   </bookViews>
@@ -508,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -564,9 +564,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1398,6 +1395,517 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>40 ft/s</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'L-D Ratio'!$A$3:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'L-D Ratio'!$J$3:$J$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1.2422733819434713</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1500149315094266</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2387505790918491</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.782255055793609</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7617843162380324</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5728098489166618</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4739313189885286</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1310114580951864</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.98415016316278803</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.77662318892531512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.64310147366945369</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.5614896681257131</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.48406490455376938</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.40163489331785002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9720-3D44-B4E4-B6B43A92F010}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>100 ft/s</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'L-D Ratio'!$A$3:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'L-D Ratio'!$K$3:$K$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>-16.966385829856982</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.3893318538787574</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.50814721428748499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3218014285369324</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4542822854526913</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.9333366782973216</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0136433995282621</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5768250294376491</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.2897046865296318</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0030238976013233</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.7224313166350149</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5643764310734365</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.4032121630892371</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2933842881583335</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9720-3D44-B4E4-B6B43A92F010}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="11316096"/>
+        <c:axId val="1415700672"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="11316096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1415700672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1415700672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="11316096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -6090,6 +6598,692 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>C_M</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs Angle of Attack </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>40 ft_s: 2.4 in</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'40 ft '!$P$24:$P$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>-4.0709042000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.9768829000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.4004100000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0190073900000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0295488800000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.92998504</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0007105500000009</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.0275877</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.9743014</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.0581964</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.997199500000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17.959525500000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20.004430599999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22.034937899999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'40 ft '!$P$40:$P$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>-1.3733299999999962E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.6367139999999971E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.0108809999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.0761926000000021E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3.1229654000000037E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-3.3525134000000095E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-3.210054400000012E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2.9960280000000117E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2.2550090000000134E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2.2808964000000154E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1.9174594000000156E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-2.0828904000000148E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-2.010125200000018E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2.0755096000000195E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-451B-4224-ADC0-0F9F99F0DD29}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>100 ft_s: 2.3 in</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'40 ft '!$P$24:$P$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>-4.0709042000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.9768829000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.4004100000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0190073900000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0295488800000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.92998504</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0007105500000009</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.0275877</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.9743014</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.0581964</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.997199500000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17.959525500000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20.004430599999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22.034937899999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'40 ft '!$Q$40:$Q$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>-7.1574199999997479E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.0025409999999855E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.8697819999999973E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5.5443573000000107E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-7.5805431000000256E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-7.2630244000000399E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-6.1107005000000658E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-3.8910371000000499E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.8467634000000732E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3435209999994608E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.2363386999999282E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.4463399999992177E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.8348939999994762E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.4353479999993422E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-451B-4224-ADC0-0F9F99F0DD29}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1282341967"/>
+        <c:axId val="1282339887"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1282341967"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Angle of Attack (degrees)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1282339887"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1282339887"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>C_M</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1282341967"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>Neutral Moment vs Angle of Attack</a:t>
             </a:r>
           </a:p>
@@ -8905,7 +10099,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -9527,7 +10721,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -10179,7 +11373,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -10715,7 +11909,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -11226,518 +12420,47 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>40 ft/s</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'L-D Ratio'!$A$3:$A$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>22</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'L-D Ratio'!$J$3:$J$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>1.2422733819434713</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.1500149315094266</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.2387505790918491</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.782255055793609</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.7617843162380324</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.5728098489166618</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.4739313189885286</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.1310114580951864</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.98415016316278803</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.77662318892531512</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.64310147366945369</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.5614896681257131</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.48406490455376938</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.40163489331785002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9720-3D44-B4E4-B6B43A92F010}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>100 ft/s</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'L-D Ratio'!$A$3:$A$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>22</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'L-D Ratio'!$K$3:$K$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>-16.966385829856982</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-5.3893318538787574</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.50814721428748499</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.3218014285369324</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.4542822854526913</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.9333366782973216</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.0136433995282621</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.5768250294376491</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.2897046865296318</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.0030238976013233</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.7224313166350149</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.5643764310734365</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.4032121630892371</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.2933842881583335</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-9720-3D44-B4E4-B6B43A92F010}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="11316096"/>
-        <c:axId val="1415700672"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="11316096"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1415700672"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1415700672"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="11316096"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -12098,6 +12821,522 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -16822,16 +18061,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>97970</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>87086</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>544284</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>141515</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>206829</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>87085</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16856,6 +18095,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>707571</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>32657</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>326572</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E93C37EC-430A-D072-5C46-995B4D12B7F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -16864,15 +18139,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>499110</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:colOff>529590</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>167640</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18379,23 +19654,23 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="31"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="30"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
@@ -19201,8 +20476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBB9CFD-C2AD-D349-8BB0-705312183456}">
   <dimension ref="A1:AO62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AH55" sqref="AH55"/>
+    <sheetView tabSelected="1" topLeftCell="J18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -20739,24 +22014,24 @@
       </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="30"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="29"/>
       <c r="T20">
         <v>22.034937899999999</v>
       </c>
@@ -23384,25 +24659,92 @@
         <v>5.7966979999999557E-2</v>
       </c>
     </row>
+    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="P40">
+        <f>AC24</f>
+        <v>-1.3733299999999962E-2</v>
+      </c>
+      <c r="Q40">
+        <f>'100 ft'!AA4</f>
+        <v>-7.1574199999997479E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="P41">
+        <f t="shared" ref="P41:P53" si="21">AC25</f>
+        <v>-1.6367139999999971E-2</v>
+      </c>
+      <c r="Q41">
+        <f>'100 ft'!AA5</f>
+        <v>-2.0025409999999855E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="P42">
+        <f t="shared" si="21"/>
+        <v>-2.0108809999999998E-2</v>
+      </c>
+      <c r="Q42">
+        <f>'100 ft'!AA6</f>
+        <v>-3.8697819999999973E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="P43">
+        <f t="shared" si="21"/>
+        <v>-2.0761926000000021E-2</v>
+      </c>
+      <c r="Q43">
+        <f>'100 ft'!AA7</f>
+        <v>-5.5443573000000107E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="P44">
+        <f t="shared" si="21"/>
+        <v>-3.1229654000000037E-2</v>
+      </c>
+      <c r="Q44">
+        <f>'100 ft'!AA8</f>
+        <v>-7.5805431000000256E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="P45">
+        <f t="shared" si="21"/>
+        <v>-3.3525134000000095E-2</v>
+      </c>
+      <c r="Q45">
+        <f>'100 ft'!AA9</f>
+        <v>-7.2630244000000399E-2</v>
+      </c>
+    </row>
     <row r="46" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="31"/>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
-      <c r="K46" s="31"/>
-      <c r="L46" s="31"/>
-      <c r="M46" s="31"/>
-      <c r="N46" s="31"/>
-      <c r="O46" s="31"/>
-      <c r="P46" s="29"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
+      <c r="K46" s="30"/>
+      <c r="L46" s="30"/>
+      <c r="M46" s="30"/>
+      <c r="N46" s="30"/>
+      <c r="O46" s="30"/>
+      <c r="P46">
+        <f t="shared" si="21"/>
+        <v>-3.210054400000012E-2</v>
+      </c>
+      <c r="Q46">
+        <f>'100 ft'!AA10</f>
+        <v>-6.1107005000000658E-2</v>
+      </c>
     </row>
     <row r="47" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
@@ -23446,6 +24788,14 @@
       <c r="O47" t="s">
         <v>40</v>
       </c>
+      <c r="P47">
+        <f t="shared" si="21"/>
+        <v>-2.9960280000000117E-2</v>
+      </c>
+      <c r="Q47">
+        <f>'100 ft'!AA11</f>
+        <v>-3.8910371000000499E-2</v>
+      </c>
     </row>
     <row r="48" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
@@ -23489,704 +24839,752 @@
       <c r="O48" t="s">
         <v>52</v>
       </c>
+      <c r="P48">
+        <f t="shared" si="21"/>
+        <v>-2.2550090000000134E-2</v>
+      </c>
+      <c r="Q48">
+        <f>'100 ft'!AA12</f>
+        <v>-1.8467634000000732E-2</v>
+      </c>
     </row>
-    <row r="49" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C49">
-        <f t="shared" ref="C49:C62" si="21">C4*0.0254</f>
+        <f t="shared" ref="C49:C62" si="22">C4*0.0254</f>
         <v>6.3500000000000001E-2</v>
       </c>
       <c r="D49">
-        <f t="shared" ref="D49:D62" si="22">D4*6894.76</f>
+        <f t="shared" ref="D49:D62" si="23">D4*6894.76</f>
         <v>99186.524644460005</v>
       </c>
       <c r="E49">
-        <f t="shared" ref="E49:E62" si="23">E4*0.555556</f>
+        <f t="shared" ref="E49:E62" si="24">E4*0.555556</f>
         <v>296.65023732000003</v>
       </c>
       <c r="F49">
-        <f t="shared" ref="F49:F62" si="24">F4*515.379</f>
+        <f t="shared" ref="F49:F62" si="25">F4*515.379</f>
         <v>1.1651688432</v>
       </c>
       <c r="G49" s="1">
-        <f t="shared" ref="G49:G62" si="25">G4*157.087</f>
+        <f t="shared" ref="G49:G62" si="26">G4*157.087</f>
         <v>6.0007233999999997E-5</v>
       </c>
       <c r="I49">
-        <f t="shared" ref="I49:I62" si="26">I4/180*PI()</f>
+        <f t="shared" ref="I49:I62" si="27">I4/180*PI()</f>
         <v>-7.1050681823265752E-2</v>
       </c>
       <c r="J49">
-        <f t="shared" ref="J49:J62" si="27">J4*6894.76</f>
+        <f t="shared" ref="J49:J62" si="28">J4*6894.76</f>
         <v>83.418184392800001</v>
       </c>
       <c r="K49">
-        <f t="shared" ref="K49:K62" si="28">K4*0.3048</f>
+        <f t="shared" ref="K49:K62" si="29">K4*0.3048</f>
         <v>11.96605797792</v>
       </c>
       <c r="L49">
-        <f t="shared" ref="L49:L62" si="29">L4</f>
+        <f t="shared" ref="L49:L62" si="30">L4</f>
         <v>48376.863299999997</v>
       </c>
       <c r="M49">
-        <f t="shared" ref="M49:N62" si="30">M4*4.44822</f>
+        <f t="shared" ref="M49:N62" si="31">M4*4.44822</f>
         <v>-0.13627566792000001</v>
       </c>
       <c r="N49">
+        <f t="shared" si="31"/>
+        <v>-0.14662889997</v>
+      </c>
+      <c r="O49">
+        <f t="shared" ref="O49:O62" si="32">O4*0.1129848333</f>
+        <v>-7.3868467148040301E-3</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="21"/>
+        <v>-2.2808964000000154E-2</v>
+      </c>
+      <c r="Q49">
+        <f>'100 ft'!AA13</f>
+        <v>3.3435209999994608E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C50">
+        <f t="shared" si="22"/>
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="23"/>
+        <v>99186.524644460005</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="24"/>
+        <v>296.65023732000003</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="25"/>
+        <v>1.1651688432</v>
+      </c>
+      <c r="G50" s="1">
+        <f t="shared" si="26"/>
+        <v>6.0007233999999997E-5</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="27"/>
+        <v>-3.4503115531373814E-2</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="28"/>
+        <v>85.712691573200004</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="29"/>
+        <v>12.129509629680001</v>
+      </c>
+      <c r="L50">
         <f t="shared" si="30"/>
-        <v>-0.14662889997</v>
-      </c>
-      <c r="O49">
-        <f t="shared" ref="O49:O62" si="31">O4*0.1129848333</f>
-        <v>-7.3868467148040301E-3</v>
+        <v>49037.671900000001</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="31"/>
+        <v>-7.5195379812000002E-2</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="31"/>
+        <v>-8.0677810961999996E-2</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="32"/>
+        <v>-3.06888274361127E-3</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="21"/>
+        <v>-1.9174594000000156E-2</v>
+      </c>
+      <c r="Q50">
+        <f>'100 ft'!AA14</f>
+        <v>1.2363386999999282E-2</v>
       </c>
     </row>
-    <row r="50" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C50">
+    <row r="51" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C51">
+        <f t="shared" si="22"/>
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="23"/>
+        <v>99186.524644460005</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="24"/>
+        <v>296.65023732000003</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="25"/>
+        <v>1.1651688432</v>
+      </c>
+      <c r="G51" s="1">
+        <f t="shared" si="26"/>
+        <v>6.0007233999999997E-5</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="27"/>
+        <v>-5.9348350417740383E-4</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="28"/>
+        <v>86.146923557999997</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="29"/>
+        <v>12.160196131680001</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="30"/>
+        <v>49161.730499999998</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="31"/>
+        <v>-3.6161359668E-2</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="31"/>
+        <v>-8.610864276E-3</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="32"/>
+        <v>1.7470720489862371E-3</v>
+      </c>
+      <c r="P51">
         <f t="shared" si="21"/>
+        <v>-2.0828904000000148E-2</v>
+      </c>
+      <c r="Q51">
+        <f>'100 ft'!AA15</f>
+        <v>6.4463399999992177E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C52">
+        <f t="shared" si="22"/>
         <v>6.3500000000000001E-2</v>
       </c>
-      <c r="D50">
+      <c r="D52">
+        <f t="shared" si="23"/>
+        <v>99186.524644460005</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="24"/>
+        <v>296.65023732000003</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="25"/>
+        <v>1.1651688432</v>
+      </c>
+      <c r="G52" s="1">
+        <f t="shared" si="26"/>
+        <v>6.0007233999999997E-5</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="27"/>
+        <v>3.5238326577597234E-2</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="28"/>
+        <v>84.706608194000012</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="29"/>
+        <v>12.058110504</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="30"/>
+        <v>48749.015599999999</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="31"/>
+        <v>1.8839234790600002E-2</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="31"/>
+        <v>8.298359028119999E-2</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="32"/>
+        <v>7.4044644398604982E-3</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="21"/>
+        <v>-2.010125200000018E-2</v>
+      </c>
+      <c r="Q52">
+        <f>'100 ft'!AA16</f>
+        <v>1.8348939999994762E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C53">
         <f t="shared" si="22"/>
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="23"/>
         <v>99186.524644460005</v>
       </c>
-      <c r="E50">
+      <c r="E53">
+        <f t="shared" si="24"/>
+        <v>296.65023732000003</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="25"/>
+        <v>1.1651688432</v>
+      </c>
+      <c r="G53" s="1">
+        <f t="shared" si="26"/>
+        <v>6.0007233999999997E-5</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="27"/>
+        <v>7.0328895326049884E-2</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="28"/>
+        <v>84.459637890799996</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="29"/>
+        <v>12.040519703519999</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="30"/>
+        <v>48677.898399999998</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="31"/>
+        <v>7.662374773620001E-2</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="31"/>
+        <v>0.16028511329880002</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="32"/>
+        <v>1.3299461675467996E-2</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="21"/>
+        <v>-2.0755096000000195E-2</v>
+      </c>
+      <c r="Q53">
+        <f>'100 ft'!AA17</f>
+        <v>7.4353479999993422E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C54">
+        <f t="shared" si="22"/>
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="D54">
         <f t="shared" si="23"/>
+        <v>99186.524644460005</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="24"/>
         <v>296.65023732000003</v>
       </c>
-      <c r="F50">
+      <c r="F54">
+        <f t="shared" si="25"/>
+        <v>1.1651688432</v>
+      </c>
+      <c r="G54" s="1">
+        <f t="shared" si="26"/>
+        <v>6.0007233999999997E-5</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="27"/>
+        <v>0.10349776354200764</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="28"/>
+        <v>84.277960964800002</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="29"/>
+        <v>12.027564697679999</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="30"/>
+        <v>48625.523399999998</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="31"/>
+        <v>0.12544340705820001</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="31"/>
+        <v>0.25139822596979999</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="32"/>
+        <v>1.9113073675952837E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C55">
+        <f t="shared" si="22"/>
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="23"/>
+        <v>99186.524644460005</v>
+      </c>
+      <c r="E55">
         <f t="shared" si="24"/>
+        <v>296.65023732000003</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="25"/>
         <v>1.1651688432</v>
       </c>
-      <c r="G50" s="1">
+      <c r="G55" s="1">
+        <f t="shared" si="26"/>
+        <v>6.0007233999999997E-5</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="27"/>
+        <v>0.13963874159654643</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="28"/>
+        <v>83.971626778000001</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="29"/>
+        <v>12.005688104399999</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="30"/>
+        <v>48537.078099999999</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="31"/>
+        <v>0.1576609748742</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="31"/>
+        <v>0.32105245812779998</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="32"/>
+        <v>2.3198240307069278E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C56">
+        <f t="shared" si="22"/>
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="23"/>
+        <v>99186.524644460005</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="24"/>
+        <v>296.65023732000003</v>
+      </c>
+      <c r="F56">
         <f t="shared" si="25"/>
+        <v>1.1651688432</v>
+      </c>
+      <c r="G56" s="1">
+        <f t="shared" si="26"/>
         <v>6.0007233999999997E-5</v>
       </c>
-      <c r="I50">
+      <c r="I56">
+        <f t="shared" si="27"/>
+        <v>0.17501442139748538</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="28"/>
+        <v>85.500677703199997</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="29"/>
+        <v>12.114497742000001</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="30"/>
+        <v>48976.980499999998</v>
+      </c>
+      <c r="M56">
+        <f t="shared" si="31"/>
+        <v>0.23616240523679999</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="31"/>
+        <v>0.38607168952800003</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="32"/>
+        <v>2.6919996871117933E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C57">
+        <f t="shared" si="22"/>
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="23"/>
+        <v>99186.524644460005</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="24"/>
+        <v>296.65023732000003</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="25"/>
+        <v>1.1651688432</v>
+      </c>
+      <c r="G57" s="1">
         <f t="shared" si="26"/>
-        <v>-3.4503115531373814E-2</v>
-      </c>
-      <c r="J50">
+        <v>6.0007233999999997E-5</v>
+      </c>
+      <c r="I57">
         <f t="shared" si="27"/>
-        <v>85.712691573200004</v>
-      </c>
-      <c r="K50">
+        <v>0.20899098505616653</v>
+      </c>
+      <c r="J57">
         <f t="shared" si="28"/>
-        <v>12.129509629680001</v>
-      </c>
-      <c r="L50">
+        <v>86.537994345200005</v>
+      </c>
+      <c r="K57">
         <f t="shared" si="29"/>
-        <v>49037.671900000001</v>
-      </c>
-      <c r="M50">
+        <v>12.1877676996</v>
+      </c>
+      <c r="L57">
         <f t="shared" si="30"/>
-        <v>-7.5195379812000002E-2</v>
-      </c>
-      <c r="N50">
+        <v>49273.199200000003</v>
+      </c>
+      <c r="M57">
+        <f t="shared" si="31"/>
+        <v>0.29173944452520001</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="31"/>
+        <v>0.44104813015200006</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="32"/>
+        <v>2.943412295337787E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C58">
+        <f t="shared" si="22"/>
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="23"/>
+        <v>99186.524644460005</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="24"/>
+        <v>296.65023732000003</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="25"/>
+        <v>1.1651688432</v>
+      </c>
+      <c r="G58" s="1">
+        <f t="shared" si="26"/>
+        <v>6.0007233999999997E-5</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="27"/>
+        <v>0.24536181407201374</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="28"/>
+        <v>87.571243078799995</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="29"/>
+        <v>12.260307447839999</v>
+      </c>
+      <c r="L58">
         <f t="shared" si="30"/>
-        <v>-8.0677810961999996E-2</v>
-      </c>
-      <c r="O50">
+        <v>49566.464800000002</v>
+      </c>
+      <c r="M58">
         <f t="shared" si="31"/>
-        <v>-3.06888274361127E-3</v>
+        <v>0.36606937865400002</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="31"/>
+        <v>0.46673032866180003</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="32"/>
+        <v>3.102895923797569E-2</v>
       </c>
     </row>
-    <row r="51" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C51">
-        <f t="shared" si="21"/>
+    <row r="59" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C59">
+        <f t="shared" si="22"/>
         <v>6.3500000000000001E-2</v>
       </c>
-      <c r="D51">
+      <c r="D59">
+        <f t="shared" si="23"/>
+        <v>99186.524644460005</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="24"/>
+        <v>296.65023732000003</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="25"/>
+        <v>1.1651688432</v>
+      </c>
+      <c r="G59" s="1">
+        <f t="shared" si="26"/>
+        <v>6.0007233999999997E-5</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="27"/>
+        <v>0.27920380237339065</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="28"/>
+        <v>85.607822273599993</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="29"/>
+        <v>12.122087993520001</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="30"/>
+        <v>49007.664100000002</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="31"/>
+        <v>0.40980699110820001</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="31"/>
+        <v>0.46716914556479999</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="32"/>
+        <v>3.0645080838507276E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C60">
         <f t="shared" si="22"/>
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="23"/>
         <v>99186.524644460005</v>
       </c>
-      <c r="E51">
+      <c r="E60">
+        <f t="shared" si="24"/>
+        <v>296.65023732000003</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="25"/>
+        <v>1.1651688432</v>
+      </c>
+      <c r="G60" s="1">
+        <f t="shared" si="26"/>
+        <v>6.0007233999999997E-5</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="27"/>
+        <v>0.31345285207088092</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="28"/>
+        <v>84.517484927200002</v>
+      </c>
+      <c r="K60">
+        <f t="shared" si="29"/>
+        <v>12.044643891360002</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="30"/>
+        <v>48694.570299999999</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="31"/>
+        <v>0.4638061577982</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="31"/>
+        <v>0.50215194934380003</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="32"/>
+        <v>3.2964545351474639E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C61">
+        <f t="shared" si="22"/>
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="D61">
         <f t="shared" si="23"/>
+        <v>99186.524644460005</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="24"/>
         <v>296.65023732000003</v>
       </c>
-      <c r="F51">
+      <c r="F61">
+        <f t="shared" si="25"/>
+        <v>1.1651688432</v>
+      </c>
+      <c r="G61" s="1">
+        <f t="shared" si="26"/>
+        <v>6.0007233999999997E-5</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="27"/>
+        <v>0.34914317895670477</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="28"/>
+        <v>87.631985914400005</v>
+      </c>
+      <c r="K61">
+        <f t="shared" si="29"/>
+        <v>12.264563004480001</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="30"/>
+        <v>49583.667999999998</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="31"/>
+        <v>0.52808258094060001</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="31"/>
+        <v>0.54369245249340004</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="32"/>
+        <v>3.5414641798855138E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C62">
+        <f t="shared" si="22"/>
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="23"/>
+        <v>99186.524644460005</v>
+      </c>
+      <c r="E62">
         <f t="shared" si="24"/>
+        <v>296.65023732000003</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="25"/>
         <v>1.1651688432</v>
       </c>
-      <c r="G51" s="1">
-        <f t="shared" si="25"/>
+      <c r="G62" s="1">
+        <f t="shared" si="26"/>
         <v>6.0007233999999997E-5</v>
       </c>
-      <c r="I51">
-        <f t="shared" si="26"/>
-        <v>-5.9348350417740383E-4</v>
-      </c>
-      <c r="J51">
+      <c r="I62">
         <f t="shared" si="27"/>
-        <v>86.146923557999997</v>
-      </c>
-      <c r="K51">
+        <v>0.384582216827485</v>
+      </c>
+      <c r="J62">
         <f t="shared" si="28"/>
-        <v>12.160196131680001</v>
-      </c>
-      <c r="L51">
+        <v>87.180999662800005</v>
+      </c>
+      <c r="K62">
         <f t="shared" si="29"/>
-        <v>49161.730499999998</v>
-      </c>
-      <c r="M51">
+        <v>12.23296377888</v>
+      </c>
+      <c r="L62">
         <f t="shared" si="30"/>
-        <v>-3.6161359668E-2</v>
-      </c>
-      <c r="N51">
-        <f t="shared" si="30"/>
-        <v>-8.610864276E-3</v>
-      </c>
-      <c r="O51">
+        <v>49455.917999999998</v>
+      </c>
+      <c r="M62">
         <f t="shared" si="31"/>
-        <v>1.7470720489862371E-3</v>
-      </c>
-    </row>
-    <row r="52" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C52">
-        <f t="shared" si="21"/>
-        <v>6.3500000000000001E-2</v>
-      </c>
-      <c r="D52">
-        <f t="shared" si="22"/>
-        <v>99186.524644460005</v>
-      </c>
-      <c r="E52">
-        <f t="shared" si="23"/>
-        <v>296.65023732000003</v>
-      </c>
-      <c r="F52">
-        <f t="shared" si="24"/>
-        <v>1.1651688432</v>
-      </c>
-      <c r="G52" s="1">
-        <f t="shared" si="25"/>
-        <v>6.0007233999999997E-5</v>
-      </c>
-      <c r="I52">
-        <f t="shared" si="26"/>
-        <v>3.5238326577597234E-2</v>
-      </c>
-      <c r="J52">
-        <f t="shared" si="27"/>
-        <v>84.706608194000012</v>
-      </c>
-      <c r="K52">
-        <f t="shared" si="28"/>
-        <v>12.058110504</v>
-      </c>
-      <c r="L52">
-        <f t="shared" si="29"/>
-        <v>48749.015599999999</v>
-      </c>
-      <c r="M52">
-        <f t="shared" si="30"/>
-        <v>1.8839234790600002E-2</v>
-      </c>
-      <c r="N52">
-        <f t="shared" si="30"/>
-        <v>8.298359028119999E-2</v>
-      </c>
-      <c r="O52">
+        <v>0.60611165482139995</v>
+      </c>
+      <c r="N62">
         <f t="shared" si="31"/>
-        <v>7.4044644398604982E-3</v>
-      </c>
-    </row>
-    <row r="53" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C53">
-        <f t="shared" si="21"/>
-        <v>6.3500000000000001E-2</v>
-      </c>
-      <c r="D53">
-        <f t="shared" si="22"/>
-        <v>99186.524644460005</v>
-      </c>
-      <c r="E53">
-        <f t="shared" si="23"/>
-        <v>296.65023732000003</v>
-      </c>
-      <c r="F53">
-        <f t="shared" si="24"/>
-        <v>1.1651688432</v>
-      </c>
-      <c r="G53" s="1">
-        <f t="shared" si="25"/>
-        <v>6.0007233999999997E-5</v>
-      </c>
-      <c r="I53">
-        <f t="shared" si="26"/>
-        <v>7.0328895326049884E-2</v>
-      </c>
-      <c r="J53">
-        <f t="shared" si="27"/>
-        <v>84.459637890799996</v>
-      </c>
-      <c r="K53">
-        <f t="shared" si="28"/>
-        <v>12.040519703519999</v>
-      </c>
-      <c r="L53">
-        <f t="shared" si="29"/>
-        <v>48677.898399999998</v>
-      </c>
-      <c r="M53">
-        <f t="shared" si="30"/>
-        <v>7.662374773620001E-2</v>
-      </c>
-      <c r="N53">
-        <f t="shared" si="30"/>
-        <v>0.16028511329880002</v>
-      </c>
-      <c r="O53">
-        <f t="shared" si="31"/>
-        <v>1.3299461675467996E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C54">
-        <f t="shared" si="21"/>
-        <v>6.3500000000000001E-2</v>
-      </c>
-      <c r="D54">
-        <f t="shared" si="22"/>
-        <v>99186.524644460005</v>
-      </c>
-      <c r="E54">
-        <f t="shared" si="23"/>
-        <v>296.65023732000003</v>
-      </c>
-      <c r="F54">
-        <f t="shared" si="24"/>
-        <v>1.1651688432</v>
-      </c>
-      <c r="G54" s="1">
-        <f t="shared" si="25"/>
-        <v>6.0007233999999997E-5</v>
-      </c>
-      <c r="I54">
-        <f t="shared" si="26"/>
-        <v>0.10349776354200764</v>
-      </c>
-      <c r="J54">
-        <f t="shared" si="27"/>
-        <v>84.277960964800002</v>
-      </c>
-      <c r="K54">
-        <f t="shared" si="28"/>
-        <v>12.027564697679999</v>
-      </c>
-      <c r="L54">
-        <f t="shared" si="29"/>
-        <v>48625.523399999998</v>
-      </c>
-      <c r="M54">
-        <f t="shared" si="30"/>
-        <v>0.12544340705820001</v>
-      </c>
-      <c r="N54">
-        <f t="shared" si="30"/>
-        <v>0.25139822596979999</v>
-      </c>
-      <c r="O54">
-        <f t="shared" si="31"/>
-        <v>1.9113073675952837E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C55">
-        <f t="shared" si="21"/>
-        <v>6.3500000000000001E-2</v>
-      </c>
-      <c r="D55">
-        <f t="shared" si="22"/>
-        <v>99186.524644460005</v>
-      </c>
-      <c r="E55">
-        <f t="shared" si="23"/>
-        <v>296.65023732000003</v>
-      </c>
-      <c r="F55">
-        <f t="shared" si="24"/>
-        <v>1.1651688432</v>
-      </c>
-      <c r="G55" s="1">
-        <f t="shared" si="25"/>
-        <v>6.0007233999999997E-5</v>
-      </c>
-      <c r="I55">
-        <f t="shared" si="26"/>
-        <v>0.13963874159654643</v>
-      </c>
-      <c r="J55">
-        <f t="shared" si="27"/>
-        <v>83.971626778000001</v>
-      </c>
-      <c r="K55">
-        <f t="shared" si="28"/>
-        <v>12.005688104399999</v>
-      </c>
-      <c r="L55">
-        <f t="shared" si="29"/>
-        <v>48537.078099999999</v>
-      </c>
-      <c r="M55">
-        <f t="shared" si="30"/>
-        <v>0.1576609748742</v>
-      </c>
-      <c r="N55">
-        <f t="shared" si="30"/>
-        <v>0.32105245812779998</v>
-      </c>
-      <c r="O55">
-        <f t="shared" si="31"/>
-        <v>2.3198240307069278E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C56">
-        <f t="shared" si="21"/>
-        <v>6.3500000000000001E-2</v>
-      </c>
-      <c r="D56">
-        <f t="shared" si="22"/>
-        <v>99186.524644460005</v>
-      </c>
-      <c r="E56">
-        <f t="shared" si="23"/>
-        <v>296.65023732000003</v>
-      </c>
-      <c r="F56">
-        <f t="shared" si="24"/>
-        <v>1.1651688432</v>
-      </c>
-      <c r="G56" s="1">
-        <f t="shared" si="25"/>
-        <v>6.0007233999999997E-5</v>
-      </c>
-      <c r="I56">
-        <f t="shared" si="26"/>
-        <v>0.17501442139748538</v>
-      </c>
-      <c r="J56">
-        <f t="shared" si="27"/>
-        <v>85.500677703199997</v>
-      </c>
-      <c r="K56">
-        <f t="shared" si="28"/>
-        <v>12.114497742000001</v>
-      </c>
-      <c r="L56">
-        <f t="shared" si="29"/>
-        <v>48976.980499999998</v>
-      </c>
-      <c r="M56">
-        <f t="shared" si="30"/>
-        <v>0.23616240523679999</v>
-      </c>
-      <c r="N56">
-        <f t="shared" si="30"/>
-        <v>0.38607168952800003</v>
-      </c>
-      <c r="O56">
-        <f t="shared" si="31"/>
-        <v>2.6919996871117933E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C57">
-        <f t="shared" si="21"/>
-        <v>6.3500000000000001E-2</v>
-      </c>
-      <c r="D57">
-        <f t="shared" si="22"/>
-        <v>99186.524644460005</v>
-      </c>
-      <c r="E57">
-        <f t="shared" si="23"/>
-        <v>296.65023732000003</v>
-      </c>
-      <c r="F57">
-        <f t="shared" si="24"/>
-        <v>1.1651688432</v>
-      </c>
-      <c r="G57" s="1">
-        <f t="shared" si="25"/>
-        <v>6.0007233999999997E-5</v>
-      </c>
-      <c r="I57">
-        <f t="shared" si="26"/>
-        <v>0.20899098505616653</v>
-      </c>
-      <c r="J57">
-        <f t="shared" si="27"/>
-        <v>86.537994345200005</v>
-      </c>
-      <c r="K57">
-        <f t="shared" si="28"/>
-        <v>12.1877676996</v>
-      </c>
-      <c r="L57">
-        <f t="shared" si="29"/>
-        <v>49273.199200000003</v>
-      </c>
-      <c r="M57">
-        <f t="shared" si="30"/>
-        <v>0.29173944452520001</v>
-      </c>
-      <c r="N57">
-        <f t="shared" si="30"/>
-        <v>0.44104813015200006</v>
-      </c>
-      <c r="O57">
-        <f t="shared" si="31"/>
-        <v>2.943412295337787E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C58">
-        <f t="shared" si="21"/>
-        <v>6.3500000000000001E-2</v>
-      </c>
-      <c r="D58">
-        <f t="shared" si="22"/>
-        <v>99186.524644460005</v>
-      </c>
-      <c r="E58">
-        <f t="shared" si="23"/>
-        <v>296.65023732000003</v>
-      </c>
-      <c r="F58">
-        <f t="shared" si="24"/>
-        <v>1.1651688432</v>
-      </c>
-      <c r="G58" s="1">
-        <f t="shared" si="25"/>
-        <v>6.0007233999999997E-5</v>
-      </c>
-      <c r="I58">
-        <f t="shared" si="26"/>
-        <v>0.24536181407201374</v>
-      </c>
-      <c r="J58">
-        <f t="shared" si="27"/>
-        <v>87.571243078799995</v>
-      </c>
-      <c r="K58">
-        <f t="shared" si="28"/>
-        <v>12.260307447839999</v>
-      </c>
-      <c r="L58">
-        <f t="shared" si="29"/>
-        <v>49566.464800000002</v>
-      </c>
-      <c r="M58">
-        <f t="shared" si="30"/>
-        <v>0.36606937865400002</v>
-      </c>
-      <c r="N58">
-        <f t="shared" si="30"/>
-        <v>0.46673032866180003</v>
-      </c>
-      <c r="O58">
-        <f t="shared" si="31"/>
-        <v>3.102895923797569E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C59">
-        <f t="shared" si="21"/>
-        <v>6.3500000000000001E-2</v>
-      </c>
-      <c r="D59">
-        <f t="shared" si="22"/>
-        <v>99186.524644460005</v>
-      </c>
-      <c r="E59">
-        <f t="shared" si="23"/>
-        <v>296.65023732000003</v>
-      </c>
-      <c r="F59">
-        <f t="shared" si="24"/>
-        <v>1.1651688432</v>
-      </c>
-      <c r="G59" s="1">
-        <f t="shared" si="25"/>
-        <v>6.0007233999999997E-5</v>
-      </c>
-      <c r="I59">
-        <f t="shared" si="26"/>
-        <v>0.27920380237339065</v>
-      </c>
-      <c r="J59">
-        <f t="shared" si="27"/>
-        <v>85.607822273599993</v>
-      </c>
-      <c r="K59">
-        <f t="shared" si="28"/>
-        <v>12.122087993520001</v>
-      </c>
-      <c r="L59">
-        <f t="shared" si="29"/>
-        <v>49007.664100000002</v>
-      </c>
-      <c r="M59">
-        <f t="shared" si="30"/>
-        <v>0.40980699110820001</v>
-      </c>
-      <c r="N59">
-        <f t="shared" si="30"/>
-        <v>0.46716914556479999</v>
-      </c>
-      <c r="O59">
-        <f t="shared" si="31"/>
-        <v>3.0645080838507276E-2</v>
-      </c>
-    </row>
-    <row r="60" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C60">
-        <f t="shared" si="21"/>
-        <v>6.3500000000000001E-2</v>
-      </c>
-      <c r="D60">
-        <f t="shared" si="22"/>
-        <v>99186.524644460005</v>
-      </c>
-      <c r="E60">
-        <f t="shared" si="23"/>
-        <v>296.65023732000003</v>
-      </c>
-      <c r="F60">
-        <f t="shared" si="24"/>
-        <v>1.1651688432</v>
-      </c>
-      <c r="G60" s="1">
-        <f t="shared" si="25"/>
-        <v>6.0007233999999997E-5</v>
-      </c>
-      <c r="I60">
-        <f t="shared" si="26"/>
-        <v>0.31345285207088092</v>
-      </c>
-      <c r="J60">
-        <f t="shared" si="27"/>
-        <v>84.517484927200002</v>
-      </c>
-      <c r="K60">
-        <f t="shared" si="28"/>
-        <v>12.044643891360002</v>
-      </c>
-      <c r="L60">
-        <f t="shared" si="29"/>
-        <v>48694.570299999999</v>
-      </c>
-      <c r="M60">
-        <f t="shared" si="30"/>
-        <v>0.4638061577982</v>
-      </c>
-      <c r="N60">
-        <f t="shared" si="30"/>
-        <v>0.50215194934380003</v>
-      </c>
-      <c r="O60">
-        <f t="shared" si="31"/>
-        <v>3.2964545351474639E-2</v>
-      </c>
-    </row>
-    <row r="61" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C61">
-        <f t="shared" si="21"/>
-        <v>6.3500000000000001E-2</v>
-      </c>
-      <c r="D61">
-        <f t="shared" si="22"/>
-        <v>99186.524644460005</v>
-      </c>
-      <c r="E61">
-        <f t="shared" si="23"/>
-        <v>296.65023732000003</v>
-      </c>
-      <c r="F61">
-        <f t="shared" si="24"/>
-        <v>1.1651688432</v>
-      </c>
-      <c r="G61" s="1">
-        <f t="shared" si="25"/>
-        <v>6.0007233999999997E-5</v>
-      </c>
-      <c r="I61">
-        <f t="shared" si="26"/>
-        <v>0.34914317895670477</v>
-      </c>
-      <c r="J61">
-        <f t="shared" si="27"/>
-        <v>87.631985914400005</v>
-      </c>
-      <c r="K61">
-        <f t="shared" si="28"/>
-        <v>12.264563004480001</v>
-      </c>
-      <c r="L61">
-        <f t="shared" si="29"/>
-        <v>49583.667999999998</v>
-      </c>
-      <c r="M61">
-        <f t="shared" si="30"/>
-        <v>0.52808258094060001</v>
-      </c>
-      <c r="N61">
-        <f t="shared" si="30"/>
-        <v>0.54369245249340004</v>
-      </c>
-      <c r="O61">
-        <f t="shared" si="31"/>
-        <v>3.5414641798855138E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C62">
-        <f t="shared" si="21"/>
-        <v>6.3500000000000001E-2</v>
-      </c>
-      <c r="D62">
-        <f t="shared" si="22"/>
-        <v>99186.524644460005</v>
-      </c>
-      <c r="E62">
-        <f t="shared" si="23"/>
-        <v>296.65023732000003</v>
-      </c>
-      <c r="F62">
-        <f t="shared" si="24"/>
-        <v>1.1651688432</v>
-      </c>
-      <c r="G62" s="1">
-        <f t="shared" si="25"/>
-        <v>6.0007233999999997E-5</v>
-      </c>
-      <c r="I62">
-        <f t="shared" si="26"/>
-        <v>0.384582216827485</v>
-      </c>
-      <c r="J62">
-        <f t="shared" si="27"/>
-        <v>87.180999662800005</v>
-      </c>
-      <c r="K62">
-        <f t="shared" si="28"/>
-        <v>12.23296377888</v>
-      </c>
-      <c r="L62">
-        <f t="shared" si="29"/>
-        <v>49455.917999999998</v>
-      </c>
-      <c r="M62">
-        <f t="shared" si="30"/>
-        <v>0.60611165482139995</v>
-      </c>
-      <c r="N62">
-        <f t="shared" si="30"/>
         <v>0.58362185484119999</v>
       </c>
       <c r="O62">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>3.7922613597245219E-2</v>
       </c>
     </row>
@@ -24204,8 +25602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23BC9146-1D19-EA45-93B1-07300A05A5AC}">
   <dimension ref="A1:AO56"/>
   <sheetViews>
-    <sheetView topLeftCell="P12" workbookViewId="0">
-      <selection activeCell="AA34" sqref="AA34"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -26482,23 +27880,23 @@
       </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
-      <c r="O20" s="32"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
       <c r="V20">
         <v>-2.0466473000000001</v>
       </c>
@@ -27549,23 +28947,23 @@
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="31"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
-      <c r="K40" s="31"/>
-      <c r="L40" s="31"/>
-      <c r="M40" s="31"/>
-      <c r="N40" s="31"/>
-      <c r="O40" s="31"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
+      <c r="K40" s="30"/>
+      <c r="L40" s="30"/>
+      <c r="M40" s="30"/>
+      <c r="N40" s="30"/>
+      <c r="O40" s="30"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
@@ -28374,18 +29772,18 @@
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="33" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="35"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="34"/>
     </row>
     <row r="2" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
@@ -28955,18 +30353,18 @@
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="36" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="38"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="37"/>
     </row>
     <row r="2" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
@@ -29529,7 +30927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F31448C-E105-E445-85D7-EC0F84352834}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScale="89" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="89" workbookViewId="0">
       <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
@@ -29540,18 +30938,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="36" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="38"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="37"/>
     </row>
     <row r="2" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
@@ -30101,11 +31499,11 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
@@ -30154,22 +31552,22 @@
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="33" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="33" t="s">
+      <c r="E1" s="34"/>
+      <c r="F1" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="33" t="s">
+      <c r="G1" s="34"/>
+      <c r="H1" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="35"/>
+      <c r="I1" s="34"/>
       <c r="J1" s="13" t="s">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
C_m tabulated highlight values
</commit_message>
<xml_diff>
--- a/Lab 6/neutral moment update.xlsx
+++ b/Lab 6/neutral moment update.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\ae460\lab05_06\AE-460\Lab 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E828FE-3350-4098-BA99-312707622990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7667A938-A4A4-4D5E-9DF5-00F8D9651D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7DB2D3F6-6F86-4E49-8BA8-4E3C7F5D5D0B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="90">
   <si>
     <t>Data Point</t>
   </si>
@@ -306,6 +306,9 @@
   <si>
     <t>Initial Guess:</t>
   </si>
+  <si>
+    <t>C_M values</t>
+  </si>
 </sst>
 </file>
 
@@ -328,7 +331,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -338,6 +341,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -508,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -593,6 +602,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18061,16 +18071,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>87086</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>337457</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>206829</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>391886</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>87085</xdr:rowOff>
+      <xdr:rowOff>195942</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18097,16 +18107,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>707571</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>32657</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>163285</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>326572</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>163285</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>315685</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>87085</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20476,8 +20486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBB9CFD-C2AD-D349-8BB0-705312183456}">
   <dimension ref="A1:AO62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView tabSelected="1" topLeftCell="J27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R41" sqref="R41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -24659,62 +24669,67 @@
         <v>5.7966979999999557E-2</v>
       </c>
     </row>
+    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="P39" t="s">
+        <v>89</v>
+      </c>
+    </row>
     <row r="40" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="P40">
+      <c r="P40" s="38">
         <f>AC24</f>
         <v>-1.3733299999999962E-2</v>
       </c>
-      <c r="Q40">
+      <c r="Q40" s="38">
         <f>'100 ft'!AA4</f>
         <v>-7.1574199999997479E-3</v>
       </c>
     </row>
     <row r="41" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="P41">
+      <c r="P41" s="38">
         <f t="shared" ref="P41:P53" si="21">AC25</f>
         <v>-1.6367139999999971E-2</v>
       </c>
-      <c r="Q41">
+      <c r="Q41" s="38">
         <f>'100 ft'!AA5</f>
         <v>-2.0025409999999855E-2</v>
       </c>
     </row>
     <row r="42" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="P42">
+      <c r="P42" s="38">
         <f t="shared" si="21"/>
         <v>-2.0108809999999998E-2</v>
       </c>
-      <c r="Q42">
+      <c r="Q42" s="38">
         <f>'100 ft'!AA6</f>
         <v>-3.8697819999999973E-2</v>
       </c>
     </row>
     <row r="43" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="P43">
+      <c r="P43" s="38">
         <f t="shared" si="21"/>
         <v>-2.0761926000000021E-2</v>
       </c>
-      <c r="Q43">
+      <c r="Q43" s="38">
         <f>'100 ft'!AA7</f>
         <v>-5.5443573000000107E-2</v>
       </c>
     </row>
     <row r="44" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="P44">
+      <c r="P44" s="38">
         <f t="shared" si="21"/>
         <v>-3.1229654000000037E-2</v>
       </c>
-      <c r="Q44">
+      <c r="Q44" s="38">
         <f>'100 ft'!AA8</f>
         <v>-7.5805431000000256E-2</v>
       </c>
     </row>
     <row r="45" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="P45">
+      <c r="P45" s="38">
         <f t="shared" si="21"/>
         <v>-3.3525134000000095E-2</v>
       </c>
-      <c r="Q45">
+      <c r="Q45" s="38">
         <f>'100 ft'!AA9</f>
         <v>-7.2630244000000399E-2</v>
       </c>
@@ -24737,11 +24752,11 @@
       <c r="M46" s="30"/>
       <c r="N46" s="30"/>
       <c r="O46" s="30"/>
-      <c r="P46">
+      <c r="P46" s="38">
         <f t="shared" si="21"/>
         <v>-3.210054400000012E-2</v>
       </c>
-      <c r="Q46">
+      <c r="Q46" s="38">
         <f>'100 ft'!AA10</f>
         <v>-6.1107005000000658E-2</v>
       </c>
@@ -24788,11 +24803,11 @@
       <c r="O47" t="s">
         <v>40</v>
       </c>
-      <c r="P47">
+      <c r="P47" s="38">
         <f t="shared" si="21"/>
         <v>-2.9960280000000117E-2</v>
       </c>
-      <c r="Q47">
+      <c r="Q47" s="38">
         <f>'100 ft'!AA11</f>
         <v>-3.8910371000000499E-2</v>
       </c>
@@ -24839,11 +24854,11 @@
       <c r="O48" t="s">
         <v>52</v>
       </c>
-      <c r="P48">
+      <c r="P48" s="38">
         <f t="shared" si="21"/>
         <v>-2.2550090000000134E-2</v>
       </c>
-      <c r="Q48">
+      <c r="Q48" s="38">
         <f>'100 ft'!AA12</f>
         <v>-1.8467634000000732E-2</v>
       </c>
@@ -24897,11 +24912,11 @@
         <f t="shared" ref="O49:O62" si="32">O4*0.1129848333</f>
         <v>-7.3868467148040301E-3</v>
       </c>
-      <c r="P49">
+      <c r="P49" s="38">
         <f t="shared" si="21"/>
         <v>-2.2808964000000154E-2</v>
       </c>
-      <c r="Q49">
+      <c r="Q49" s="38">
         <f>'100 ft'!AA13</f>
         <v>3.3435209999994608E-3</v>
       </c>
@@ -24955,11 +24970,11 @@
         <f t="shared" si="32"/>
         <v>-3.06888274361127E-3</v>
       </c>
-      <c r="P50">
+      <c r="P50" s="38">
         <f t="shared" si="21"/>
         <v>-1.9174594000000156E-2</v>
       </c>
-      <c r="Q50">
+      <c r="Q50" s="38">
         <f>'100 ft'!AA14</f>
         <v>1.2363386999999282E-2</v>
       </c>
@@ -25013,11 +25028,11 @@
         <f t="shared" si="32"/>
         <v>1.7470720489862371E-3</v>
       </c>
-      <c r="P51">
+      <c r="P51" s="38">
         <f t="shared" si="21"/>
         <v>-2.0828904000000148E-2</v>
       </c>
-      <c r="Q51">
+      <c r="Q51" s="38">
         <f>'100 ft'!AA15</f>
         <v>6.4463399999992177E-3</v>
       </c>
@@ -25071,11 +25086,11 @@
         <f t="shared" si="32"/>
         <v>7.4044644398604982E-3</v>
       </c>
-      <c r="P52">
+      <c r="P52" s="38">
         <f t="shared" si="21"/>
         <v>-2.010125200000018E-2</v>
       </c>
-      <c r="Q52">
+      <c r="Q52" s="38">
         <f>'100 ft'!AA16</f>
         <v>1.8348939999994762E-3</v>
       </c>
@@ -25129,11 +25144,11 @@
         <f t="shared" si="32"/>
         <v>1.3299461675467996E-2</v>
       </c>
-      <c r="P53">
+      <c r="P53" s="38">
         <f t="shared" si="21"/>
         <v>-2.0755096000000195E-2</v>
       </c>
-      <c r="Q53">
+      <c r="Q53" s="38">
         <f>'100 ft'!AA17</f>
         <v>7.4353479999993422E-3</v>
       </c>

</xml_diff>